<commit_message>
Uploading Gen2 Piat Math
</commit_message>
<xml_diff>
--- a/VariableStaging/Outcomes.xlsx
+++ b/VariableStaging/Outcomes.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gen2Weight" sheetId="1" r:id="rId1"/>
+    <sheet name="PiatMath" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>VariableCode</t>
   </si>
@@ -70,6 +71,123 @@
   </si>
   <si>
     <t>Y2544900</t>
+  </si>
+  <si>
+    <t>C0579900</t>
+  </si>
+  <si>
+    <t>C0580000</t>
+  </si>
+  <si>
+    <t>C0580100</t>
+  </si>
+  <si>
+    <t>C0799400</t>
+  </si>
+  <si>
+    <t>C0799500</t>
+  </si>
+  <si>
+    <t>C0799600</t>
+  </si>
+  <si>
+    <t>C0998600</t>
+  </si>
+  <si>
+    <t>C0998700</t>
+  </si>
+  <si>
+    <t>C0998800</t>
+  </si>
+  <si>
+    <t>C1198600</t>
+  </si>
+  <si>
+    <t>C1198700</t>
+  </si>
+  <si>
+    <t>C1198800</t>
+  </si>
+  <si>
+    <t>C1507600</t>
+  </si>
+  <si>
+    <t>C1507700</t>
+  </si>
+  <si>
+    <t>C1507800</t>
+  </si>
+  <si>
+    <t>C1564500</t>
+  </si>
+  <si>
+    <t>C1564600</t>
+  </si>
+  <si>
+    <t>C1564700</t>
+  </si>
+  <si>
+    <t>C1799900</t>
+  </si>
+  <si>
+    <t>C1800000</t>
+  </si>
+  <si>
+    <t>C1800100</t>
+  </si>
+  <si>
+    <t>C2503500</t>
+  </si>
+  <si>
+    <t>C2503600</t>
+  </si>
+  <si>
+    <t>C2503700</t>
+  </si>
+  <si>
+    <t>C2532000</t>
+  </si>
+  <si>
+    <t>C2532100</t>
+  </si>
+  <si>
+    <t>C2532200</t>
+  </si>
+  <si>
+    <t>C2802800</t>
+  </si>
+  <si>
+    <t>C2802900</t>
+  </si>
+  <si>
+    <t>C2803000</t>
+  </si>
+  <si>
+    <t>C3111300</t>
+  </si>
+  <si>
+    <t>C3111400</t>
+  </si>
+  <si>
+    <t>C3111500</t>
+  </si>
+  <si>
+    <t>C3615000</t>
+  </si>
+  <si>
+    <t>C3615100</t>
+  </si>
+  <si>
+    <t>C3615200</t>
+  </si>
+  <si>
+    <t>C3993600</t>
+  </si>
+  <si>
+    <t>C3993700</t>
+  </si>
+  <si>
+    <t>C3993800</t>
   </si>
 </sst>
 </file>
@@ -416,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +586,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1">
         <v>1994</v>
@@ -494,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1">
         <v>1998</v>
@@ -520,7 +638,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1">
         <v>2000</v>
@@ -546,7 +664,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1">
         <v>2002</v>
@@ -572,7 +690,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1">
         <v>2004</v>
@@ -598,7 +716,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1">
         <v>2006</v>
@@ -624,7 +742,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1">
         <v>2008</v>
@@ -650,7 +768,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" s="1">
         <v>2010</v>
@@ -978,4 +1096,1077 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="10" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1">
+        <v>511</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1986</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1">
+        <v>512</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1986</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <v>513</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1986</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>511</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1">
+        <v>512</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1">
+        <v>513</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
+        <v>511</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1990</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1">
+        <v>512</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>13</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1990</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1">
+        <v>513</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1990</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1">
+        <v>511</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1992</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1">
+        <v>512</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1992</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>513</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1992</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1">
+        <v>511</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1994</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1">
+        <v>512</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1994</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1">
+        <v>513</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1994</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1">
+        <v>511</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>13</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1996</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="1">
+        <v>512</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>13</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1996</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="1">
+        <v>513</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1996</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="1">
+        <v>511</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1998</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1">
+        <v>512</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>13</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1998</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1">
+        <v>513</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>13</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1998</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1">
+        <v>511</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>13</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1">
+        <v>512</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>13</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1">
+        <v>513</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>13</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="1">
+        <v>511</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>13</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="1">
+        <v>512</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>13</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="1">
+        <v>513</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>13</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="1">
+        <v>511</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1">
+        <v>13</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2004</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="1">
+        <v>512</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>13</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2004</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="1">
+        <v>513</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>13</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2004</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="1">
+        <v>511</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>13</v>
+      </c>
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="1">
+        <v>512</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>13</v>
+      </c>
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="1">
+        <v>513</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1">
+        <v>13</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="1">
+        <v>511</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>13</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>2008</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="1">
+        <v>512</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1">
+        <v>13</v>
+      </c>
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2008</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="1">
+        <v>513</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>13</v>
+      </c>
+      <c r="F37" s="1">
+        <v>2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2008</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="1">
+        <v>511</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1">
+        <v>2</v>
+      </c>
+      <c r="G38" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="1">
+        <v>512</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2</v>
+      </c>
+      <c r="E39" s="1">
+        <v>13</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2</v>
+      </c>
+      <c r="G39" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="1">
+        <v>513</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>13</v>
+      </c>
+      <c r="F40" s="1">
+        <v>2</v>
+      </c>
+      <c r="G40" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>